<commit_message>
just noticed i had pasted comments from a javascript convert into the .cpp. put them in the right file instead. The xlsx were just background research stuff.
</commit_message>
<xml_diff>
--- a/tracker/wspr_calc_direct_shift.xlsx
+++ b/tracker/wspr_calc_direct_shift.xlsx
@@ -8,7 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="orig" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="mfsk16" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="mfsk16_pll2" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="44">
   <si>
     <t xml:space="preserve">Note how it’s independent of the u4b frequency bin within the band.</t>
   </si>
@@ -109,23 +111,7 @@
     <t xml:space="preserve">shown by:</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">https://groups.io/g/QRPLabs/topic/si5351a_issues_with_frequency/96467329</t>
-    </r>
+    <t xml:space="preserve">  https://groups.io/g/QRPLabs/topic/si5351a_issues_with_frequency/96467329</t>
   </si>
   <si>
     <t xml:space="preserve">groups.io</t>
@@ -162,21 +148,29 @@
   </si>
   <si>
     <t xml:space="preserve"> and then I have manipulated b directly to send the WSPR signals. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mfsk16 shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">450 mhz pll target works on 10m!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
   <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -198,21 +192,24 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,25 +219,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFB66C"/>
-        <bgColor rgb="FFFFAA95"/>
+        <bgColor rgb="FFFF99CC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFAFD095"/>
         <bgColor rgb="FF99CCFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFAA95"/>
-        <bgColor rgb="FFFFA6A6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFA6A6"/>
-        <bgColor rgb="FFFFAA95"/>
       </patternFill>
     </fill>
   </fills>
@@ -278,52 +263,60 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -359,7 +352,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFFAA95"/>
+      <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -375,7 +368,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFFA6A6"/>
+      <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFB66C"/>
       <rgbColor rgb="FF3366FF"/>
@@ -512,444 +505,444 @@
   </sheetPr>
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J14" activeCellId="0" sqref="J14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.69"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="1"/>
+      <c r="L2" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="0" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="n">
+      <c r="D4" s="4" t="n">
         <v>26000000</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="F4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="3" t="n">
+      <c r="D5" s="4" t="n">
         <f aca="false">12000/8192</f>
         <v>1.46484375</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="F5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="3" t="n">
+      <c r="D6" s="4" t="n">
         <v>1048575</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="0" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="3" t="n">
-        <v>32</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="4" t="n">
         <v>36</v>
       </c>
-      <c r="G7" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="3" t="n">
-        <v>42</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="3" t="n">
-        <v>50</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L7" s="3" t="n">
-        <v>64</v>
-      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="0" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="3" t="n">
-        <v>34</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="D8" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="3" t="n">
-        <v>34</v>
-      </c>
-      <c r="G8" s="0" t="s">
+      <c r="F8" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="H8" s="3" t="n">
-        <v>34</v>
-      </c>
-      <c r="I8" s="0" t="s">
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="I8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="3" t="n">
-        <v>34</v>
-      </c>
-      <c r="K8" s="0" t="s">
+      <c r="J8" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="3" t="n">
-        <v>34</v>
+      <c r="L8" s="4" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="3" t="n">
+      <c r="D9" s="4" t="n">
         <f aca="false">(D8+1) * D4</f>
-        <v>910000000</v>
-      </c>
-      <c r="E9" s="0" t="s">
+        <v>520000000</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="4" t="n">
         <f aca="false">(F8+1) * D4</f>
-        <v>910000000</v>
-      </c>
-      <c r="G9" s="0" t="s">
+        <v>520000000</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="3" t="n">
+      <c r="H9" s="4" t="n">
         <f aca="false">(H8+1) * D4</f>
-        <v>910000000</v>
-      </c>
-      <c r="I9" s="0" t="s">
+        <v>520000000</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="3" t="n">
+      <c r="J9" s="4" t="n">
         <f aca="false">(J8+1) * D4</f>
-        <v>910000000</v>
-      </c>
-      <c r="K9" s="0" t="s">
+        <v>520000000</v>
+      </c>
+      <c r="K9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="3" t="n">
+      <c r="L9" s="4" t="n">
         <f aca="false">(L8+1) * D4</f>
-        <v>910000000</v>
+        <v>520000000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="3" t="n">
+      <c r="D10" s="4" t="n">
         <f aca="false">D8*D4</f>
-        <v>884000000</v>
-      </c>
-      <c r="E10" s="0" t="s">
+        <v>494000000</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="3" t="n">
+      <c r="F10" s="4" t="n">
         <f aca="false">F8*D4</f>
-        <v>884000000</v>
-      </c>
-      <c r="G10" s="0" t="s">
+        <v>494000000</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="3" t="n">
+      <c r="H10" s="4" t="n">
         <f aca="false">H8 * D4</f>
-        <v>884000000</v>
-      </c>
-      <c r="I10" s="0" t="s">
+        <v>494000000</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="3" t="n">
+      <c r="J10" s="4" t="n">
         <f aca="false">J8*D4</f>
-        <v>884000000</v>
-      </c>
-      <c r="K10" s="0" t="s">
+        <v>494000000</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="3" t="n">
+      <c r="L10" s="4" t="n">
         <f aca="false">L8*D4</f>
-        <v>884000000</v>
+        <v>494000000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G11" s="4"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="K12" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D13" s="5" t="n">
+      <c r="D13" s="6" t="n">
         <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
-        <v>554666.666666667</v>
-      </c>
-      <c r="E13" s="0" t="n">
+        <v>986074.074074074</v>
+      </c>
+      <c r="E13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F13" s="6" t="n">
         <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
-        <v>493037.037037037</v>
-      </c>
-      <c r="G13" s="0" t="n">
+        <v>887466.666666667</v>
+      </c>
+      <c r="G13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H13" s="7" t="n">
+      <c r="H13" s="6" t="n">
         <f aca="false">MIN((D4/H7)/D5, D6)</f>
-        <v>422603.174603175</v>
-      </c>
-      <c r="I13" s="0" t="n">
+        <v>739555.555555556</v>
+      </c>
+      <c r="I13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="J13" s="6" t="n">
         <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
-        <v>354986.666666667</v>
-      </c>
-      <c r="K13" s="0" t="n">
+        <v>633904.761904762</v>
+      </c>
+      <c r="K13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="L13" s="8" t="n">
+      <c r="L13" s="6" t="n">
         <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
-        <v>277333.333333333</v>
+        <v>493037.037037037</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D14" s="6" t="n">
+      <c r="D14" s="7" t="n">
         <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
         <v>1048575</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F14" s="5" t="n">
+      <c r="F14" s="8" t="n">
         <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="8" t="n">
+        <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="8" t="n">
+        <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
+        <v>1048575</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" s="7" t="n">
+        <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
         <v>986074.074074074</v>
       </c>
-      <c r="G14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="H14" s="5" t="n">
-        <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
-        <v>845206.349206349</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="J14" s="5" t="n">
-        <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
-        <v>709973.333333333</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="L14" s="6" t="n">
-        <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
-        <v>554666.666666667</v>
-      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D15" s="6" t="n">
+      <c r="D15" s="7" t="n">
         <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
         <v>1048575</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="6" t="n">
+      <c r="F15" s="7" t="n">
         <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
-        <v>59652.2666666667</v>
-      </c>
-      <c r="G15" s="0" t="n">
+        <v>107374.08</v>
+      </c>
+      <c r="G15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="6" t="n">
+      <c r="H15" s="7" t="n">
         <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
         <v>1048575</v>
       </c>
-      <c r="I15" s="0" t="n">
+      <c r="I15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="J15" s="9" t="n">
+      <c r="J15" s="8" t="n">
         <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
         <v>1048575</v>
       </c>
-      <c r="K15" s="0" t="n">
+      <c r="K15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="5" t="n">
+      <c r="L15" s="8" t="n">
         <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
-        <v>832000</v>
+        <v>1048575</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J22" s="10" t="s">
+      <c r="J22" s="9" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E29" s="0" t="s">
+      <c r="E29" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E30" s="0" t="s">
+      <c r="E30" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="0" t="s">
+      <c r="D32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11" t="s">
+      <c r="F32" s="10"/>
+      <c r="G32" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="H32" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="I32" s="11" t="s">
+      <c r="I32" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="J32" s="11" t="s">
+      <c r="J32" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K32" s="11" t="s">
+      <c r="K32" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="L32" s="11" t="n">
+      <c r="L32" s="10" t="n">
         <v>96467329</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E33" s="0" t="s">
+      <c r="E33" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E34" s="0" t="s">
+      <c r="E34" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E35" s="0" t="s">
+      <c r="E35" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E36" s="0" t="s">
+      <c r="E36" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E37" s="0" t="s">
+      <c r="E37" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E38" s="0" t="s">
+      <c r="E38" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E39" s="0" t="s">
+      <c r="E39" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -966,7 +959,7 @@
     <mergeCell ref="E32:L32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E32" r:id="rId1" display="https://groups.io/g/QRPLabs/topic/si5351a_issues_with_frequency/96467329"/>
+    <hyperlink ref="E32" r:id="rId1" display="  https://groups.io/g/QRPLabs/topic/si5351a_issues_with_frequency/96467329"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -976,4 +969,952 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>15.625</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>1048575</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>42</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <f aca="false">(D8+1) * D4</f>
+        <v>910000000</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <f aca="false">(F8+1) * D4</f>
+        <v>910000000</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <f aca="false">(H8+1) * D4</f>
+        <v>910000000</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="4" t="n">
+        <f aca="false">(J8+1) * D4</f>
+        <v>910000000</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <f aca="false">(L8+1) * D4</f>
+        <v>910000000</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <f aca="false">D8*D4</f>
+        <v>884000000</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <f aca="false">F8*D4</f>
+        <v>884000000</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <f aca="false">H8 * D4</f>
+        <v>884000000</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <f aca="false">J8*D4</f>
+        <v>884000000</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="4" t="n">
+        <f aca="false">L8*D4</f>
+        <v>884000000</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
+        <v>52000</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="12" t="n">
+        <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
+        <v>46222.2222222222</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12" t="n">
+        <f aca="false">MIN((D4/H7)/D5, D6)</f>
+        <v>39619.0476190476</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="12" t="n">
+        <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
+        <v>33280</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="12" t="n">
+        <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="12" t="n">
+        <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
+        <v>104000</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="11" t="n">
+        <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
+        <v>92444.4444444445</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="11" t="n">
+        <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
+        <v>79238.0952380952</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="11" t="n">
+        <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
+        <v>66560</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" s="12" t="n">
+        <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" s="12" t="n">
+        <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
+        <v>156000</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="12" t="n">
+        <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
+        <v>5592.4</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="12" t="n">
+        <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
+        <v>118857.142857143</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J15" s="12" t="n">
+        <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
+        <v>99840</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" s="11" t="n">
+        <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J22" s="9"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L32" s="10" t="n">
+        <v>96467329</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E32:L32"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E32" r:id="rId1" display="  https://groups.io/g/QRPLabs/topic/si5351a_issues_with_frequency/96467329"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:L39"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.67"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="n">
+        <v>26000000</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="4" t="n">
+        <v>15.625</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>1048575</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="n">
+        <v>42</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" s="4" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="4" t="n">
+        <f aca="false">(D8+1) * D4</f>
+        <v>520000000</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <f aca="false">(F8+1) * D4</f>
+        <v>910000000</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <f aca="false">(H8+1) * D4</f>
+        <v>910000000</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" s="4" t="n">
+        <f aca="false">(J8+1) * D4</f>
+        <v>910000000</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <f aca="false">(L8+1) * D4</f>
+        <v>910000000</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <f aca="false">D8*D4</f>
+        <v>494000000</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <f aca="false">F8*D4</f>
+        <v>884000000</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <f aca="false">H8 * D4</f>
+        <v>884000000</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="4" t="n">
+        <f aca="false">J8*D4</f>
+        <v>884000000</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="4" t="n">
+        <f aca="false">L8*D4</f>
+        <v>884000000</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="13" t="n">
+        <f aca="false">MIN(1*(D4/D7)/D5, D6)</f>
+        <v>92444.4444444445</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7" t="n">
+        <f aca="false">MIN(1*(D4/F7)/D5, D6)</f>
+        <v>46222.2222222222</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <f aca="false">MIN((D4/H7)/D5, D6)</f>
+        <v>39619.0476190476</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7" t="n">
+        <f aca="false">MIN(1*(D4/J7)/D5, D6)</f>
+        <v>33280</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="7" t="n">
+        <f aca="false">MIN(1*(D4/L7)/D5, D6)</f>
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" s="7" t="n">
+        <f aca="false">MIN(2*(D4/D7) / D5, D6)</f>
+        <v>184888.888888889</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="13" t="n">
+        <f aca="false">MIN(2*(D4/F7)/D5, D6)</f>
+        <v>92444.4444444445</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="13" t="n">
+        <f aca="false">MIN(2*(D4/H7)/D5, D6)</f>
+        <v>79238.0952380952</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="13" t="n">
+        <f aca="false">MIN(2*(D4/J7)/D5,D6)</f>
+        <v>66560</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" s="7" t="n">
+        <f aca="false">MIN(2*(D4/L7)/D5, D6)</f>
+        <v>52000</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <f aca="false">MIN(3*(D4/D7)/D5, D6)</f>
+        <v>277333.333333333</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <f aca="false">MIN(3*(D6/F7)/D5, D6)</f>
+        <v>5592.4</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <f aca="false">MIN(3*(D4/H7)/D5, D6)</f>
+        <v>118857.142857143</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J15" s="7" t="n">
+        <f aca="false">MIN(3*(D4/J7)/D5, D6)</f>
+        <v>99840</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" s="13" t="n">
+        <f aca="false">MIN(3*(D4/L7)/D5,D6)</f>
+        <v>78000</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="7"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D21" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J22" s="9"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="L32" s="10" t="n">
+        <v>96467329</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E37" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E38" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E39" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="E32:L32"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E32" r:id="rId1" display="  https://groups.io/g/QRPLabs/topic/si5351a_issues_with_frequency/96467329"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>